<commit_message>
add offer gender in binary
</commit_message>
<xml_diff>
--- a/_static/global/binaryrankings/workers_rank_mat.xlsx
+++ b/_static/global/binaryrankings/workers_rank_mat.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="67">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -25,6 +25,9 @@
     <t>index</t>
   </si>
   <si>
+    <t>prolificid</t>
+  </si>
+  <si>
     <t>name</t>
   </si>
   <si>
@@ -43,10 +46,85 @@
     <t>mat_range</t>
   </si>
   <si>
+    <t>60bd88b8fc436774352f53b9</t>
+  </si>
+  <si>
+    <t>5c5882fc5bfe7600011197cb</t>
+  </si>
+  <si>
+    <t>5c0e89c6c323400001e6c4a5</t>
+  </si>
+  <si>
+    <t>60b45e9961dd412bfb6780f8</t>
+  </si>
+  <si>
+    <t>608b14a312c099ac00b721b6</t>
+  </si>
+  <si>
+    <t>60cb36ee9f58331a33cf5506</t>
+  </si>
+  <si>
+    <t>6036f9b3b1842f8b659b18c7</t>
+  </si>
+  <si>
+    <t>60d5775a99b502eec8cf56b4</t>
+  </si>
+  <si>
+    <t>5e96194b0a9fe909389e9f7b</t>
+  </si>
+  <si>
+    <t>6077db0613ce87b4a62a78f9</t>
+  </si>
+  <si>
+    <t>60bfcf5805c5ae12a546f9f3</t>
+  </si>
+  <si>
+    <t>60c0e5899d387663c07eb3a4</t>
+  </si>
+  <si>
+    <t>5e2522d6b734b47915f88275</t>
+  </si>
+  <si>
+    <t>601d69a993d94008fb2b25dc</t>
+  </si>
+  <si>
+    <t>60db4fde6193c50664c9c478</t>
+  </si>
+  <si>
+    <t>5dd671942b033b5ec8bc97b4</t>
+  </si>
+  <si>
+    <t>5ff8ad350d084e10f500e48a</t>
+  </si>
+  <si>
+    <t>60b83826821417f8e484a207</t>
+  </si>
+  <si>
+    <t>60b322994d0b901954690036</t>
+  </si>
+  <si>
+    <t>60bf9943e4e04642d4634ecc</t>
+  </si>
+  <si>
+    <t>60c2341fe95d71ee52c043f0</t>
+  </si>
+  <si>
+    <t>60b091ed11ccda59e3fc7761</t>
+  </si>
+  <si>
+    <t>6088fc724afd5c008db33e9d</t>
+  </si>
+  <si>
+    <t>6097b95056caf5ebb2720002</t>
+  </si>
+  <si>
+    <t>Annes</t>
+  </si>
+  <si>
     <t>Colleen</t>
   </si>
   <si>
-    <t>Annes</t>
+    <t>Bri</t>
   </si>
   <si>
     <t>Jewel</t>
@@ -55,24 +133,21 @@
     <t>Khushi</t>
   </si>
   <si>
-    <t>Bri</t>
+    <t>Shaniek</t>
+  </si>
+  <si>
+    <t>Kellie</t>
   </si>
   <si>
     <t>Shadaisia</t>
   </si>
   <si>
-    <t>Kellie</t>
-  </si>
-  <si>
-    <t>Shaniek</t>
+    <t>Tina</t>
   </si>
   <si>
     <t>Lori</t>
   </si>
   <si>
-    <t>Tina</t>
-  </si>
-  <si>
     <t>Giana</t>
   </si>
   <si>
@@ -91,12 +166,12 @@
     <t>Juan</t>
   </si>
   <si>
+    <t>Drew</t>
+  </si>
+  <si>
     <t>Eli</t>
   </si>
   <si>
-    <t>Drew</t>
-  </si>
-  <si>
     <t>Brennan</t>
   </si>
   <si>
@@ -121,10 +196,10 @@
     <t>male</t>
   </si>
   <si>
+    <t>Asian</t>
+  </si>
+  <si>
     <t>White</t>
-  </si>
-  <si>
-    <t>Asian</t>
   </si>
   <si>
     <t>Black or African American</t>
@@ -497,13 +572,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -531,8 +606,11 @@
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -543,28 +621,31 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2">
-        <v>13.41179440177212</v>
-      </c>
-      <c r="H2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2">
+        <v>34</v>
+      </c>
+      <c r="G2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2">
+        <v>13.44015278694422</v>
+      </c>
+      <c r="I2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2">
         <v>1</v>
       </c>
-      <c r="J2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -575,28 +656,31 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3">
-        <v>13.28345529631224</v>
-      </c>
-      <c r="H3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3">
+        <v>35</v>
+      </c>
+      <c r="G3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3">
+        <v>13.26073009200145</v>
+      </c>
+      <c r="I3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3">
         <v>2</v>
       </c>
-      <c r="J3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="K3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -607,28 +691,31 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4">
-        <v>8.23763560135623</v>
-      </c>
-      <c r="H4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I4">
+        <v>36</v>
+      </c>
+      <c r="G4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4">
+        <v>8.354532088468041</v>
+      </c>
+      <c r="I4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4">
         <v>3</v>
       </c>
-      <c r="J4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="K4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -639,28 +726,31 @@
         <v>3</v>
       </c>
       <c r="D5">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5">
-        <v>8.166612813012238</v>
-      </c>
-      <c r="H5" t="s">
-        <v>36</v>
-      </c>
-      <c r="I5">
+        <v>37</v>
+      </c>
+      <c r="G5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5">
+        <v>8.098102820749885</v>
+      </c>
+      <c r="I5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J5">
         <v>4</v>
       </c>
-      <c r="J5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="K5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -671,28 +761,31 @@
         <v>4</v>
       </c>
       <c r="D6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6">
-        <v>8.005597717419404</v>
-      </c>
-      <c r="H6" t="s">
-        <v>37</v>
-      </c>
-      <c r="I6">
+        <v>38</v>
+      </c>
+      <c r="G6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6">
+        <v>8.097338185867613</v>
+      </c>
+      <c r="I6" t="s">
+        <v>60</v>
+      </c>
+      <c r="J6">
         <v>5</v>
       </c>
-      <c r="J6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="K6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -703,28 +796,31 @@
         <v>5</v>
       </c>
       <c r="D7">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7">
-        <v>5.361927025870195</v>
-      </c>
-      <c r="H7" t="s">
-        <v>37</v>
-      </c>
-      <c r="I7">
+        <v>39</v>
+      </c>
+      <c r="G7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7">
+        <v>5.483549169353528</v>
+      </c>
+      <c r="I7" t="s">
+        <v>62</v>
+      </c>
+      <c r="J7">
         <v>6</v>
       </c>
-      <c r="J7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="K7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -738,25 +834,28 @@
         <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8">
-        <v>5.237683582040133</v>
-      </c>
-      <c r="H8" t="s">
-        <v>35</v>
-      </c>
-      <c r="I8">
+        <v>40</v>
+      </c>
+      <c r="G8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8">
+        <v>5.36924149709817</v>
+      </c>
+      <c r="I8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J8">
         <v>7</v>
       </c>
-      <c r="J8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="K8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -767,28 +866,31 @@
         <v>7</v>
       </c>
       <c r="D9">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9">
-        <v>5.010962683506764</v>
-      </c>
-      <c r="H9" t="s">
-        <v>37</v>
-      </c>
-      <c r="I9">
+        <v>41</v>
+      </c>
+      <c r="G9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9">
+        <v>5.049422940202584</v>
+      </c>
+      <c r="I9" t="s">
+        <v>62</v>
+      </c>
+      <c r="J9">
         <v>8</v>
       </c>
-      <c r="J9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="K9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -799,28 +901,31 @@
         <v>8</v>
       </c>
       <c r="D10">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10">
-        <v>4.477479880056773</v>
-      </c>
-      <c r="H10" t="s">
-        <v>35</v>
-      </c>
-      <c r="I10">
+        <v>42</v>
+      </c>
+      <c r="G10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10">
+        <v>4.105146646021751</v>
+      </c>
+      <c r="I10" t="s">
+        <v>61</v>
+      </c>
+      <c r="J10">
         <v>9</v>
       </c>
-      <c r="J10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="K10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -831,28 +936,31 @@
         <v>9</v>
       </c>
       <c r="D11">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11">
-        <v>4.389849861394186</v>
-      </c>
-      <c r="H11" t="s">
-        <v>35</v>
-      </c>
-      <c r="I11">
+        <v>43</v>
+      </c>
+      <c r="G11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11">
+        <v>4.050914323979571</v>
+      </c>
+      <c r="I11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J11">
         <v>10</v>
       </c>
-      <c r="J11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="K11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -866,25 +974,28 @@
         <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F12" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12">
-        <v>2.382527936458554</v>
-      </c>
-      <c r="H12" t="s">
-        <v>35</v>
-      </c>
-      <c r="I12">
+        <v>44</v>
+      </c>
+      <c r="G12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12">
+        <v>2.435214467044919</v>
+      </c>
+      <c r="I12" t="s">
+        <v>61</v>
+      </c>
+      <c r="J12">
         <v>11</v>
       </c>
-      <c r="J12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="K12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -898,25 +1009,28 @@
         <v>44</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F13" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13">
-        <v>1.029173221199296</v>
-      </c>
-      <c r="H13" t="s">
-        <v>36</v>
-      </c>
-      <c r="I13">
+        <v>45</v>
+      </c>
+      <c r="G13" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13">
+        <v>1.191712437135525</v>
+      </c>
+      <c r="I13" t="s">
+        <v>60</v>
+      </c>
+      <c r="J13">
         <v>12</v>
       </c>
-      <c r="J13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="K13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -930,25 +1044,28 @@
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F14" t="s">
-        <v>34</v>
-      </c>
-      <c r="G14">
-        <v>14.2745467615059</v>
-      </c>
-      <c r="H14" t="s">
-        <v>35</v>
-      </c>
-      <c r="I14">
+        <v>46</v>
+      </c>
+      <c r="G14" t="s">
+        <v>59</v>
+      </c>
+      <c r="H14">
+        <v>14.40027434213815</v>
+      </c>
+      <c r="I14" t="s">
+        <v>61</v>
+      </c>
+      <c r="J14">
         <v>1</v>
       </c>
-      <c r="J14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="K14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -962,25 +1079,28 @@
         <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F15" t="s">
-        <v>34</v>
-      </c>
-      <c r="G15">
-        <v>13.07194186949775</v>
-      </c>
-      <c r="H15" t="s">
-        <v>37</v>
-      </c>
-      <c r="I15">
+        <v>47</v>
+      </c>
+      <c r="G15" t="s">
+        <v>59</v>
+      </c>
+      <c r="H15">
+        <v>13.3019045588994</v>
+      </c>
+      <c r="I15" t="s">
+        <v>62</v>
+      </c>
+      <c r="J15">
         <v>2</v>
       </c>
-      <c r="J15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="K15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -994,25 +1114,28 @@
         <v>22</v>
       </c>
       <c r="E16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F16" t="s">
-        <v>34</v>
-      </c>
-      <c r="G16">
-        <v>8.189927172263737</v>
-      </c>
-      <c r="H16" t="s">
-        <v>37</v>
-      </c>
-      <c r="I16">
+        <v>48</v>
+      </c>
+      <c r="G16" t="s">
+        <v>59</v>
+      </c>
+      <c r="H16">
+        <v>8.361239919308625</v>
+      </c>
+      <c r="I16" t="s">
+        <v>62</v>
+      </c>
+      <c r="J16">
         <v>3</v>
       </c>
-      <c r="J16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="K16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1026,25 +1149,28 @@
         <v>26</v>
       </c>
       <c r="E17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F17" t="s">
-        <v>34</v>
-      </c>
-      <c r="G17">
-        <v>7.39607034879652</v>
-      </c>
-      <c r="H17" t="s">
-        <v>38</v>
-      </c>
-      <c r="I17">
+        <v>49</v>
+      </c>
+      <c r="G17" t="s">
+        <v>59</v>
+      </c>
+      <c r="H17">
+        <v>7.001638653657909</v>
+      </c>
+      <c r="I17" t="s">
+        <v>63</v>
+      </c>
+      <c r="J17">
         <v>4</v>
       </c>
-      <c r="J17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="K17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1055,28 +1181,31 @@
         <v>4</v>
       </c>
       <c r="D18">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F18" t="s">
-        <v>34</v>
-      </c>
-      <c r="G18">
-        <v>6.323612713011084</v>
-      </c>
-      <c r="H18" t="s">
-        <v>35</v>
-      </c>
-      <c r="I18">
+        <v>50</v>
+      </c>
+      <c r="G18" t="s">
+        <v>59</v>
+      </c>
+      <c r="H18">
+        <v>6.38247157770629</v>
+      </c>
+      <c r="I18" t="s">
+        <v>61</v>
+      </c>
+      <c r="J18">
         <v>5</v>
       </c>
-      <c r="J18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="K18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1087,28 +1216,31 @@
         <v>5</v>
       </c>
       <c r="D19">
+        <v>29</v>
+      </c>
+      <c r="E19" t="s">
         <v>27</v>
       </c>
-      <c r="E19" t="s">
-        <v>26</v>
-      </c>
       <c r="F19" t="s">
-        <v>34</v>
-      </c>
-      <c r="G19">
-        <v>6.252130279629233</v>
-      </c>
-      <c r="H19" t="s">
-        <v>35</v>
-      </c>
-      <c r="I19">
+        <v>51</v>
+      </c>
+      <c r="G19" t="s">
+        <v>59</v>
+      </c>
+      <c r="H19">
+        <v>6.166501710522055</v>
+      </c>
+      <c r="I19" t="s">
+        <v>61</v>
+      </c>
+      <c r="J19">
         <v>6</v>
       </c>
-      <c r="J19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="K19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1122,25 +1254,28 @@
         <v>33</v>
       </c>
       <c r="E20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F20" t="s">
-        <v>34</v>
-      </c>
-      <c r="G20">
-        <v>5.331365905335693</v>
-      </c>
-      <c r="H20" t="s">
-        <v>35</v>
-      </c>
-      <c r="I20">
+        <v>52</v>
+      </c>
+      <c r="G20" t="s">
+        <v>59</v>
+      </c>
+      <c r="H20">
+        <v>5.482491394747845</v>
+      </c>
+      <c r="I20" t="s">
+        <v>61</v>
+      </c>
+      <c r="J20">
         <v>7</v>
       </c>
-      <c r="J20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
+      <c r="K20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1154,25 +1289,28 @@
         <v>32</v>
       </c>
       <c r="E21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F21" t="s">
-        <v>34</v>
-      </c>
-      <c r="G21">
-        <v>5.299930968965304</v>
-      </c>
-      <c r="H21" t="s">
-        <v>37</v>
-      </c>
-      <c r="I21">
+        <v>53</v>
+      </c>
+      <c r="G21" t="s">
+        <v>59</v>
+      </c>
+      <c r="H21">
+        <v>5.47701608724167</v>
+      </c>
+      <c r="I21" t="s">
+        <v>62</v>
+      </c>
+      <c r="J21">
         <v>8</v>
       </c>
-      <c r="J21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="K21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1186,25 +1324,28 @@
         <v>30</v>
       </c>
       <c r="E22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F22" t="s">
-        <v>34</v>
-      </c>
-      <c r="G22">
-        <v>5.024612660958182</v>
-      </c>
-      <c r="H22" t="s">
-        <v>35</v>
-      </c>
-      <c r="I22">
+        <v>54</v>
+      </c>
+      <c r="G22" t="s">
+        <v>59</v>
+      </c>
+      <c r="H22">
+        <v>5.11301045113269</v>
+      </c>
+      <c r="I22" t="s">
+        <v>61</v>
+      </c>
+      <c r="J22">
         <v>9</v>
       </c>
-      <c r="J22" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="K22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1218,25 +1359,28 @@
         <v>44</v>
       </c>
       <c r="E23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F23" t="s">
-        <v>34</v>
-      </c>
-      <c r="G23">
-        <v>3.207723512647401</v>
-      </c>
-      <c r="H23" t="s">
-        <v>37</v>
-      </c>
-      <c r="I23">
+        <v>55</v>
+      </c>
+      <c r="G23" t="s">
+        <v>59</v>
+      </c>
+      <c r="H23">
+        <v>3.317147241751798</v>
+      </c>
+      <c r="I23" t="s">
+        <v>62</v>
+      </c>
+      <c r="J23">
         <v>10</v>
       </c>
-      <c r="J23" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="K23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1250,25 +1394,28 @@
         <v>49</v>
       </c>
       <c r="E24" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F24" t="s">
-        <v>34</v>
-      </c>
-      <c r="G24">
-        <v>1.345698146888841</v>
-      </c>
-      <c r="H24" t="s">
-        <v>36</v>
-      </c>
-      <c r="I24">
+        <v>56</v>
+      </c>
+      <c r="G24" t="s">
+        <v>59</v>
+      </c>
+      <c r="H24">
+        <v>1.019206744813832</v>
+      </c>
+      <c r="I24" t="s">
+        <v>60</v>
+      </c>
+      <c r="J24">
         <v>11</v>
       </c>
-      <c r="J24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
+      <c r="K24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1282,22 +1429,25 @@
         <v>50</v>
       </c>
       <c r="E25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F25" t="s">
-        <v>34</v>
-      </c>
-      <c r="G25">
-        <v>0.1471275131748038</v>
-      </c>
-      <c r="H25" t="s">
-        <v>37</v>
-      </c>
-      <c r="I25">
+        <v>57</v>
+      </c>
+      <c r="G25" t="s">
+        <v>59</v>
+      </c>
+      <c r="H25">
+        <v>0.2975636940466398</v>
+      </c>
+      <c r="I25" t="s">
+        <v>62</v>
+      </c>
+      <c r="J25">
         <v>12</v>
       </c>
-      <c r="J25" t="s">
-        <v>41</v>
+      <c r="K25" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
include no rank decision in binary
</commit_message>
<xml_diff>
--- a/_static/global/binaryrankings/workers_rank_mat.xlsx
+++ b/_static/global/binaryrankings/workers_rank_mat.xlsx
@@ -46,10 +46,13 @@
     <t>mat_range</t>
   </si>
   <si>
+    <t>5c5882fc5bfe7600011197cb</t>
+  </si>
+  <si>
     <t>60bd88b8fc436774352f53b9</t>
   </si>
   <si>
-    <t>5c5882fc5bfe7600011197cb</t>
+    <t>608b14a312c099ac00b721b6</t>
   </si>
   <si>
     <t>5c0e89c6c323400001e6c4a5</t>
@@ -58,9 +61,6 @@
     <t>60b45e9961dd412bfb6780f8</t>
   </si>
   <si>
-    <t>608b14a312c099ac00b721b6</t>
-  </si>
-  <si>
     <t>60cb36ee9f58331a33cf5506</t>
   </si>
   <si>
@@ -100,12 +100,12 @@
     <t>60b83826821417f8e484a207</t>
   </si>
   <si>
+    <t>60bf9943e4e04642d4634ecc</t>
+  </si>
+  <si>
     <t>60b322994d0b901954690036</t>
   </si>
   <si>
-    <t>60bf9943e4e04642d4634ecc</t>
-  </si>
-  <si>
     <t>60c2341fe95d71ee52c043f0</t>
   </si>
   <si>
@@ -118,10 +118,13 @@
     <t>6097b95056caf5ebb2720002</t>
   </si>
   <si>
+    <t>Colleen</t>
+  </si>
+  <si>
     <t>Annes</t>
   </si>
   <si>
-    <t>Colleen</t>
+    <t>Khushi</t>
   </si>
   <si>
     <t>Bri</t>
@@ -130,9 +133,6 @@
     <t>Jewel</t>
   </si>
   <si>
-    <t>Khushi</t>
-  </si>
-  <si>
     <t>Shaniek</t>
   </si>
   <si>
@@ -172,12 +172,12 @@
     <t>Eli</t>
   </si>
   <si>
+    <t>Jamarii</t>
+  </si>
+  <si>
     <t>Brennan</t>
   </si>
   <si>
-    <t>Jamarii</t>
-  </si>
-  <si>
     <t>Matthew</t>
   </si>
   <si>
@@ -196,10 +196,10 @@
     <t>male</t>
   </si>
   <si>
+    <t>White</t>
+  </si>
+  <si>
     <t>Asian</t>
-  </si>
-  <si>
-    <t>White</t>
   </si>
   <si>
     <t>Black or African American</t>
@@ -621,7 +621,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -633,7 +633,7 @@
         <v>58</v>
       </c>
       <c r="H2">
-        <v>13.44015278694422</v>
+        <v>13.42119510329043</v>
       </c>
       <c r="I2" t="s">
         <v>60</v>
@@ -656,7 +656,7 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -668,7 +668,7 @@
         <v>58</v>
       </c>
       <c r="H3">
-        <v>13.26073009200145</v>
+        <v>13.17773416771519</v>
       </c>
       <c r="I3" t="s">
         <v>61</v>
@@ -691,7 +691,7 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
@@ -703,10 +703,10 @@
         <v>58</v>
       </c>
       <c r="H4">
-        <v>8.354532088468041</v>
+        <v>8.277947983434146</v>
       </c>
       <c r="I4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J4">
         <v>3</v>
@@ -726,7 +726,7 @@
         <v>3</v>
       </c>
       <c r="D5">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
@@ -738,7 +738,7 @@
         <v>58</v>
       </c>
       <c r="H5">
-        <v>8.098102820749885</v>
+        <v>8.218874334828817</v>
       </c>
       <c r="I5" t="s">
         <v>62</v>
@@ -761,7 +761,7 @@
         <v>4</v>
       </c>
       <c r="D6">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
@@ -773,10 +773,10 @@
         <v>58</v>
       </c>
       <c r="H6">
-        <v>8.097338185867613</v>
+        <v>8.21192345112825</v>
       </c>
       <c r="I6" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J6">
         <v>5</v>
@@ -808,7 +808,7 @@
         <v>58</v>
       </c>
       <c r="H7">
-        <v>5.483549169353528</v>
+        <v>5.441970684512863</v>
       </c>
       <c r="I7" t="s">
         <v>62</v>
@@ -843,10 +843,10 @@
         <v>58</v>
       </c>
       <c r="H8">
-        <v>5.36924149709817</v>
+        <v>5.381459162249058</v>
       </c>
       <c r="I8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J8">
         <v>7</v>
@@ -878,7 +878,7 @@
         <v>58</v>
       </c>
       <c r="H9">
-        <v>5.049422940202584</v>
+        <v>5.321845954194636</v>
       </c>
       <c r="I9" t="s">
         <v>62</v>
@@ -913,10 +913,10 @@
         <v>58</v>
       </c>
       <c r="H10">
-        <v>4.105146646021751</v>
+        <v>4.498467056693604</v>
       </c>
       <c r="I10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J10">
         <v>9</v>
@@ -948,10 +948,10 @@
         <v>58</v>
       </c>
       <c r="H11">
-        <v>4.050914323979571</v>
+        <v>4.222996349665409</v>
       </c>
       <c r="I11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J11">
         <v>10</v>
@@ -983,10 +983,10 @@
         <v>58</v>
       </c>
       <c r="H12">
-        <v>2.435214467044919</v>
+        <v>2.390791975163696</v>
       </c>
       <c r="I12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J12">
         <v>11</v>
@@ -1018,10 +1018,10 @@
         <v>58</v>
       </c>
       <c r="H13">
-        <v>1.191712437135525</v>
+        <v>1.089220531548616</v>
       </c>
       <c r="I13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J13">
         <v>12</v>
@@ -1053,10 +1053,10 @@
         <v>59</v>
       </c>
       <c r="H14">
-        <v>14.40027434213815</v>
+        <v>14.11239547175637</v>
       </c>
       <c r="I14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J14">
         <v>1</v>
@@ -1088,7 +1088,7 @@
         <v>59</v>
       </c>
       <c r="H15">
-        <v>13.3019045588994</v>
+        <v>13.09487473480318</v>
       </c>
       <c r="I15" t="s">
         <v>62</v>
@@ -1123,7 +1123,7 @@
         <v>59</v>
       </c>
       <c r="H16">
-        <v>8.361239919308625</v>
+        <v>8.22111200880744</v>
       </c>
       <c r="I16" t="s">
         <v>62</v>
@@ -1158,7 +1158,7 @@
         <v>59</v>
       </c>
       <c r="H17">
-        <v>7.001638653657909</v>
+        <v>7.429121582096163</v>
       </c>
       <c r="I17" t="s">
         <v>63</v>
@@ -1193,10 +1193,10 @@
         <v>59</v>
       </c>
       <c r="H18">
-        <v>6.38247157770629</v>
+        <v>6.324528075904071</v>
       </c>
       <c r="I18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J18">
         <v>5</v>
@@ -1228,10 +1228,10 @@
         <v>59</v>
       </c>
       <c r="H19">
-        <v>6.166501710522055</v>
+        <v>6.243826188088984</v>
       </c>
       <c r="I19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J19">
         <v>6</v>
@@ -1251,7 +1251,7 @@
         <v>6</v>
       </c>
       <c r="D20">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E20" t="s">
         <v>28</v>
@@ -1263,10 +1263,10 @@
         <v>59</v>
       </c>
       <c r="H20">
-        <v>5.482491394747845</v>
+        <v>5.27722767756892</v>
       </c>
       <c r="I20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J20">
         <v>7</v>
@@ -1286,7 +1286,7 @@
         <v>7</v>
       </c>
       <c r="D21">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E21" t="s">
         <v>29</v>
@@ -1298,10 +1298,10 @@
         <v>59</v>
       </c>
       <c r="H21">
-        <v>5.47701608724167</v>
+        <v>5.186042016282854</v>
       </c>
       <c r="I21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J21">
         <v>8</v>
@@ -1333,10 +1333,10 @@
         <v>59</v>
       </c>
       <c r="H22">
-        <v>5.11301045113269</v>
+        <v>5.141087836715284</v>
       </c>
       <c r="I22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J22">
         <v>9</v>
@@ -1368,7 +1368,7 @@
         <v>59</v>
       </c>
       <c r="H23">
-        <v>3.317147241751798</v>
+        <v>3.417079858592328</v>
       </c>
       <c r="I23" t="s">
         <v>62</v>
@@ -1403,10 +1403,10 @@
         <v>59</v>
       </c>
       <c r="H24">
-        <v>1.019206744813832</v>
+        <v>1.153463192899035</v>
       </c>
       <c r="I24" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J24">
         <v>11</v>
@@ -1438,7 +1438,7 @@
         <v>59</v>
       </c>
       <c r="H25">
-        <v>0.2975636940466398</v>
+        <v>0.3269558257719956</v>
       </c>
       <c r="I25" t="s">
         <v>62</v>

</xml_diff>

<commit_message>
add infobox to make instructions for ranking easier/less
</commit_message>
<xml_diff>
--- a/_static/global/binaryrankings/workers_rank_mat.xlsx
+++ b/_static/global/binaryrankings/workers_rank_mat.xlsx
@@ -64,12 +64,12 @@
     <t>60cb36ee9f58331a33cf5506</t>
   </si>
   <si>
+    <t>60d5775a99b502eec8cf56b4</t>
+  </si>
+  <si>
     <t>6036f9b3b1842f8b659b18c7</t>
   </si>
   <si>
-    <t>60d5775a99b502eec8cf56b4</t>
-  </si>
-  <si>
     <t>5e96194b0a9fe909389e9f7b</t>
   </si>
   <si>
@@ -100,15 +100,15 @@
     <t>60b83826821417f8e484a207</t>
   </si>
   <si>
+    <t>60c2341fe95d71ee52c043f0</t>
+  </si>
+  <si>
     <t>60bf9943e4e04642d4634ecc</t>
   </si>
   <si>
     <t>60b322994d0b901954690036</t>
   </si>
   <si>
-    <t>60c2341fe95d71ee52c043f0</t>
-  </si>
-  <si>
     <t>60b091ed11ccda59e3fc7761</t>
   </si>
   <si>
@@ -136,12 +136,12 @@
     <t>Shaniek</t>
   </si>
   <si>
+    <t>Shadaisia</t>
+  </si>
+  <si>
     <t>Kellie</t>
   </si>
   <si>
-    <t>Shadaisia</t>
-  </si>
-  <si>
     <t>Tina</t>
   </si>
   <si>
@@ -172,13 +172,13 @@
     <t>Eli</t>
   </si>
   <si>
+    <t>Matthew</t>
+  </si>
+  <si>
     <t>Jamarii</t>
   </si>
   <si>
     <t>Brennan</t>
-  </si>
-  <si>
-    <t>Matthew</t>
   </si>
   <si>
     <t>Myles</t>
@@ -633,7 +633,7 @@
         <v>58</v>
       </c>
       <c r="H2">
-        <v>13.42119510329043</v>
+        <v>13.25581603006527</v>
       </c>
       <c r="I2" t="s">
         <v>60</v>
@@ -668,7 +668,7 @@
         <v>58</v>
       </c>
       <c r="H3">
-        <v>13.17773416771519</v>
+        <v>13.03564410204013</v>
       </c>
       <c r="I3" t="s">
         <v>61</v>
@@ -703,7 +703,7 @@
         <v>58</v>
       </c>
       <c r="H4">
-        <v>8.277947983434146</v>
+        <v>8.387878449008936</v>
       </c>
       <c r="I4" t="s">
         <v>61</v>
@@ -738,7 +738,7 @@
         <v>58</v>
       </c>
       <c r="H5">
-        <v>8.218874334828817</v>
+        <v>8.356292063322577</v>
       </c>
       <c r="I5" t="s">
         <v>62</v>
@@ -773,7 +773,7 @@
         <v>58</v>
       </c>
       <c r="H6">
-        <v>8.21192345112825</v>
+        <v>8.180015286402934</v>
       </c>
       <c r="I6" t="s">
         <v>62</v>
@@ -808,7 +808,7 @@
         <v>58</v>
       </c>
       <c r="H7">
-        <v>5.441970684512863</v>
+        <v>5.393336665672788</v>
       </c>
       <c r="I7" t="s">
         <v>62</v>
@@ -831,7 +831,7 @@
         <v>6</v>
       </c>
       <c r="D8">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s">
         <v>16</v>
@@ -843,10 +843,10 @@
         <v>58</v>
       </c>
       <c r="H8">
-        <v>5.381459162249058</v>
+        <v>5.339669197139461</v>
       </c>
       <c r="I8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J8">
         <v>7</v>
@@ -866,7 +866,7 @@
         <v>7</v>
       </c>
       <c r="D9">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E9" t="s">
         <v>17</v>
@@ -878,10 +878,10 @@
         <v>58</v>
       </c>
       <c r="H9">
-        <v>5.321845954194636</v>
+        <v>5.108019693417147</v>
       </c>
       <c r="I9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J9">
         <v>8</v>
@@ -913,7 +913,7 @@
         <v>58</v>
       </c>
       <c r="H10">
-        <v>4.498467056693604</v>
+        <v>4.268640122598316</v>
       </c>
       <c r="I10" t="s">
         <v>60</v>
@@ -948,7 +948,7 @@
         <v>58</v>
       </c>
       <c r="H11">
-        <v>4.222996349665409</v>
+        <v>4.254495598246366</v>
       </c>
       <c r="I11" t="s">
         <v>60</v>
@@ -983,7 +983,7 @@
         <v>58</v>
       </c>
       <c r="H12">
-        <v>2.390791975163696</v>
+        <v>2.420025270519735</v>
       </c>
       <c r="I12" t="s">
         <v>60</v>
@@ -1018,7 +1018,7 @@
         <v>58</v>
       </c>
       <c r="H13">
-        <v>1.089220531548616</v>
+        <v>1.496024677253027</v>
       </c>
       <c r="I13" t="s">
         <v>61</v>
@@ -1053,7 +1053,7 @@
         <v>59</v>
       </c>
       <c r="H14">
-        <v>14.11239547175637</v>
+        <v>14.35604799398173</v>
       </c>
       <c r="I14" t="s">
         <v>60</v>
@@ -1088,7 +1088,7 @@
         <v>59</v>
       </c>
       <c r="H15">
-        <v>13.09487473480318</v>
+        <v>13.17756464437572</v>
       </c>
       <c r="I15" t="s">
         <v>62</v>
@@ -1123,7 +1123,7 @@
         <v>59</v>
       </c>
       <c r="H16">
-        <v>8.22111200880744</v>
+        <v>8.158367614863963</v>
       </c>
       <c r="I16" t="s">
         <v>62</v>
@@ -1158,7 +1158,7 @@
         <v>59</v>
       </c>
       <c r="H17">
-        <v>7.429121582096163</v>
+        <v>7.132419507397405</v>
       </c>
       <c r="I17" t="s">
         <v>63</v>
@@ -1193,7 +1193,7 @@
         <v>59</v>
       </c>
       <c r="H18">
-        <v>6.324528075904071</v>
+        <v>6.306267974076017</v>
       </c>
       <c r="I18" t="s">
         <v>60</v>
@@ -1228,7 +1228,7 @@
         <v>59</v>
       </c>
       <c r="H19">
-        <v>6.243826188088984</v>
+        <v>6.305467982787811</v>
       </c>
       <c r="I19" t="s">
         <v>60</v>
@@ -1251,7 +1251,7 @@
         <v>6</v>
       </c>
       <c r="D20">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E20" t="s">
         <v>28</v>
@@ -1263,10 +1263,10 @@
         <v>59</v>
       </c>
       <c r="H20">
-        <v>5.27722767756892</v>
+        <v>5.443833869706829</v>
       </c>
       <c r="I20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J20">
         <v>7</v>
@@ -1286,7 +1286,7 @@
         <v>7</v>
       </c>
       <c r="D21">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E21" t="s">
         <v>29</v>
@@ -1298,10 +1298,10 @@
         <v>59</v>
       </c>
       <c r="H21">
-        <v>5.186042016282854</v>
+        <v>5.210446373867417</v>
       </c>
       <c r="I21" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J21">
         <v>8</v>
@@ -1321,7 +1321,7 @@
         <v>8</v>
       </c>
       <c r="D22">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E22" t="s">
         <v>30</v>
@@ -1333,7 +1333,7 @@
         <v>59</v>
       </c>
       <c r="H22">
-        <v>5.141087836715284</v>
+        <v>5.049269166493271</v>
       </c>
       <c r="I22" t="s">
         <v>60</v>
@@ -1368,7 +1368,7 @@
         <v>59</v>
       </c>
       <c r="H23">
-        <v>3.417079858592328</v>
+        <v>3.295791998891051</v>
       </c>
       <c r="I23" t="s">
         <v>62</v>
@@ -1403,7 +1403,7 @@
         <v>59</v>
       </c>
       <c r="H24">
-        <v>1.153463192899035</v>
+        <v>1.043195326962711</v>
       </c>
       <c r="I24" t="s">
         <v>61</v>
@@ -1438,7 +1438,7 @@
         <v>59</v>
       </c>
       <c r="H25">
-        <v>0.3269558257719956</v>
+        <v>0.2516358054655306</v>
       </c>
       <c r="I25" t="s">
         <v>62</v>

</xml_diff>